<commit_message>
11/10/24 Module 3.2 Assignment: Normalized Tables
</commit_message>
<xml_diff>
--- a/module-3/trueworthy-NormalizedTables.xlsx
+++ b/module-3/trueworthy-NormalizedTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\csd\csd-310\module-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223EF048-DDA5-466D-837F-A38F8128237A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9D6EF1-340E-40BC-BF7F-F4A4658B59CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0276E738-CF3A-48AB-B662-2CA8F9A50255}"/>
   </bookViews>
@@ -606,12 +606,12 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" style="2" bestFit="1" customWidth="1"/>

</xml_diff>